<commit_message>
data: update financial plan to v12; users are counts (UI already formats correctly)
</commit_message>
<xml_diff>
--- a/public/data/consultantcloud_36m_financial_plan.xlsx
+++ b/public/data/consultantcloud_36m_financial_plan.xlsx
@@ -475,6 +475,60 @@
             </numRef>
           </val>
         </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Financial Plan'!$B$1:$AK$1</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Financial Plan'!$B$12:$AK$12</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Financial Plan'!$B$1:$AK$1</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Financial Plan'!$B$13:$AK$13</f>
+            </numRef>
+          </val>
+        </ser>
         <axId val="10"/>
         <axId val="100"/>
       </lineChart>
@@ -584,7 +638,7 @@
           </cat>
           <val>
             <numRef>
-              <f>'Financial Plan'!$B$14:$AK$14</f>
+              <f>'Financial Plan'!$B$16:$AK$16</f>
             </numRef>
           </val>
         </ser>
@@ -1013,7 +1067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1336,10 +1390,10 @@
         <v>18</v>
       </c>
       <c r="D3" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" t="n">
         <v>43</v>
@@ -1348,7 +1402,7 @@
         <v>51</v>
       </c>
       <c r="H3" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I3" t="n">
         <v>68</v>
@@ -1357,85 +1411,85 @@
         <v>76</v>
       </c>
       <c r="K3" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L3" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M3" t="n">
         <v>101</v>
       </c>
       <c r="N3" t="n">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="O3" t="n">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="P3" t="n">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="Q3" t="n">
-        <v>134</v>
+        <v>201</v>
       </c>
       <c r="R3" t="n">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="S3" t="n">
-        <v>150</v>
+        <v>226</v>
       </c>
       <c r="T3" t="n">
-        <v>159</v>
+        <v>239</v>
       </c>
       <c r="U3" t="n">
-        <v>167</v>
+        <v>251</v>
       </c>
       <c r="V3" t="n">
-        <v>175</v>
+        <v>264</v>
       </c>
       <c r="W3" t="n">
-        <v>184</v>
+        <v>276</v>
       </c>
       <c r="X3" t="n">
-        <v>192</v>
+        <v>288</v>
       </c>
       <c r="Y3" t="n">
-        <v>200</v>
+        <v>301</v>
       </c>
       <c r="Z3" t="n">
-        <v>208</v>
+        <v>418</v>
       </c>
       <c r="AA3" t="n">
-        <v>217</v>
+        <v>434</v>
       </c>
       <c r="AB3" t="n">
-        <v>225</v>
+        <v>451</v>
       </c>
       <c r="AC3" t="n">
-        <v>233</v>
+        <v>467</v>
       </c>
       <c r="AD3" t="n">
-        <v>242</v>
+        <v>484</v>
       </c>
       <c r="AE3" t="n">
-        <v>250</v>
+        <v>501</v>
       </c>
       <c r="AF3" t="n">
-        <v>258</v>
+        <v>517</v>
       </c>
       <c r="AG3" t="n">
-        <v>266</v>
+        <v>534</v>
       </c>
       <c r="AH3" t="n">
-        <v>275</v>
+        <v>550</v>
       </c>
       <c r="AI3" t="n">
-        <v>283</v>
+        <v>567</v>
       </c>
       <c r="AJ3" t="n">
-        <v>291</v>
+        <v>583</v>
       </c>
       <c r="AK3" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4">
@@ -1484,73 +1538,73 @@
         <v>200</v>
       </c>
       <c r="O4" t="n">
-        <v>218</v>
+        <v>255</v>
       </c>
       <c r="P4" t="n">
-        <v>236</v>
+        <v>309</v>
       </c>
       <c r="Q4" t="n">
-        <v>255</v>
+        <v>364</v>
       </c>
       <c r="R4" t="n">
-        <v>273</v>
+        <v>418</v>
       </c>
       <c r="S4" t="n">
-        <v>291</v>
+        <v>473</v>
       </c>
       <c r="T4" t="n">
-        <v>309</v>
+        <v>527</v>
       </c>
       <c r="U4" t="n">
-        <v>327</v>
+        <v>582</v>
       </c>
       <c r="V4" t="n">
-        <v>345</v>
+        <v>636</v>
       </c>
       <c r="W4" t="n">
-        <v>364</v>
+        <v>691</v>
       </c>
       <c r="X4" t="n">
-        <v>382</v>
+        <v>745</v>
       </c>
       <c r="Y4" t="n">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="Z4" t="n">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="AA4" t="n">
-        <v>436</v>
+        <v>909</v>
       </c>
       <c r="AB4" t="n">
-        <v>473</v>
+        <v>1018</v>
       </c>
       <c r="AC4" t="n">
-        <v>509</v>
+        <v>1127</v>
       </c>
       <c r="AD4" t="n">
-        <v>545</v>
+        <v>1236</v>
       </c>
       <c r="AE4" t="n">
-        <v>582</v>
+        <v>1345</v>
       </c>
       <c r="AF4" t="n">
-        <v>618</v>
+        <v>1455</v>
       </c>
       <c r="AG4" t="n">
-        <v>655</v>
+        <v>1564</v>
       </c>
       <c r="AH4" t="n">
-        <v>691</v>
+        <v>1673</v>
       </c>
       <c r="AI4" t="n">
-        <v>727</v>
+        <v>1782</v>
       </c>
       <c r="AJ4" t="n">
-        <v>764</v>
+        <v>1891</v>
       </c>
       <c r="AK4" t="n">
-        <v>800</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5">
@@ -1560,7 +1614,112 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>110000</v>
+        <v>50000</v>
+      </c>
+      <c r="C5" t="n">
+        <v/>
+      </c>
+      <c r="D5" t="n">
+        <v/>
+      </c>
+      <c r="E5" t="n">
+        <v/>
+      </c>
+      <c r="F5" t="n">
+        <v/>
+      </c>
+      <c r="G5" t="n">
+        <v/>
+      </c>
+      <c r="H5" t="n">
+        <v/>
+      </c>
+      <c r="I5" t="n">
+        <v/>
+      </c>
+      <c r="J5" t="n">
+        <v/>
+      </c>
+      <c r="K5" t="n">
+        <v/>
+      </c>
+      <c r="L5" t="n">
+        <v/>
+      </c>
+      <c r="M5" t="n">
+        <v/>
+      </c>
+      <c r="N5" t="n">
+        <v/>
+      </c>
+      <c r="O5" t="n">
+        <v/>
+      </c>
+      <c r="P5" t="n">
+        <v/>
+      </c>
+      <c r="Q5" t="n">
+        <v/>
+      </c>
+      <c r="R5" t="n">
+        <v/>
+      </c>
+      <c r="S5" t="n">
+        <v/>
+      </c>
+      <c r="T5" t="n">
+        <v/>
+      </c>
+      <c r="U5" t="n">
+        <v/>
+      </c>
+      <c r="V5" t="n">
+        <v/>
+      </c>
+      <c r="W5" t="n">
+        <v/>
+      </c>
+      <c r="X5" t="n">
+        <v/>
+      </c>
+      <c r="Y5" t="n">
+        <v/>
+      </c>
+      <c r="Z5" t="n">
+        <v/>
+      </c>
+      <c r="AA5" t="n">
+        <v/>
+      </c>
+      <c r="AB5" t="n">
+        <v/>
+      </c>
+      <c r="AC5" t="n">
+        <v/>
+      </c>
+      <c r="AD5" t="n">
+        <v/>
+      </c>
+      <c r="AE5" t="n">
+        <v/>
+      </c>
+      <c r="AF5" t="n">
+        <v/>
+      </c>
+      <c r="AG5" t="n">
+        <v/>
+      </c>
+      <c r="AH5" t="n">
+        <v/>
+      </c>
+      <c r="AI5" t="n">
+        <v/>
+      </c>
+      <c r="AJ5" t="n">
+        <v/>
+      </c>
+      <c r="AK5" t="n">
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -1576,10 +1735,10 @@
         <v>269.82</v>
       </c>
       <c r="D6" t="n">
-        <v>389.74</v>
+        <v>404.73</v>
       </c>
       <c r="E6" t="n">
-        <v>509.66</v>
+        <v>524.65</v>
       </c>
       <c r="F6" t="n">
         <v>644.5700000000001</v>
@@ -1588,7 +1747,7 @@
         <v>764.49</v>
       </c>
       <c r="H6" t="n">
-        <v>884.41</v>
+        <v>899.4</v>
       </c>
       <c r="I6" t="n">
         <v>1019.32</v>
@@ -1597,85 +1756,85 @@
         <v>1139.24</v>
       </c>
       <c r="K6" t="n">
-        <v>1259.16</v>
+        <v>1274.15</v>
       </c>
       <c r="L6" t="n">
-        <v>1379.08</v>
+        <v>1394.07</v>
       </c>
       <c r="M6" t="n">
         <v>1513.99</v>
       </c>
       <c r="N6" t="n">
-        <v>1633.91</v>
+        <v>2458.36</v>
       </c>
       <c r="O6" t="n">
-        <v>1753.83</v>
+        <v>2653.23</v>
       </c>
       <c r="P6" t="n">
-        <v>1888.74</v>
+        <v>2833.11</v>
       </c>
       <c r="Q6" t="n">
-        <v>2008.66</v>
+        <v>3012.99</v>
       </c>
       <c r="R6" t="n">
-        <v>2128.58</v>
+        <v>3207.86</v>
       </c>
       <c r="S6" t="n">
-        <v>2248.5</v>
+        <v>3387.74</v>
       </c>
       <c r="T6" t="n">
-        <v>2383.41</v>
+        <v>3582.61</v>
       </c>
       <c r="U6" t="n">
-        <v>2503.33</v>
+        <v>3762.49</v>
       </c>
       <c r="V6" t="n">
-        <v>2623.25</v>
+        <v>3957.36</v>
       </c>
       <c r="W6" t="n">
-        <v>2758.16</v>
+        <v>4137.24</v>
       </c>
       <c r="X6" t="n">
-        <v>2878.08</v>
+        <v>4317.12</v>
       </c>
       <c r="Y6" t="n">
-        <v>2998</v>
+        <v>4511.99</v>
       </c>
       <c r="Z6" t="n">
-        <v>3117.92</v>
+        <v>6265.82</v>
       </c>
       <c r="AA6" t="n">
-        <v>3252.83</v>
+        <v>6505.66</v>
       </c>
       <c r="AB6" t="n">
-        <v>3372.75</v>
+        <v>6760.49</v>
       </c>
       <c r="AC6" t="n">
-        <v>3492.67</v>
+        <v>7000.33</v>
       </c>
       <c r="AD6" t="n">
-        <v>3627.58</v>
+        <v>7255.16</v>
       </c>
       <c r="AE6" t="n">
-        <v>3747.5</v>
+        <v>7509.99</v>
       </c>
       <c r="AF6" t="n">
-        <v>3867.42</v>
+        <v>7749.83</v>
       </c>
       <c r="AG6" t="n">
-        <v>3987.34</v>
+        <v>8004.66</v>
       </c>
       <c r="AH6" t="n">
-        <v>4122.25</v>
+        <v>8244.5</v>
       </c>
       <c r="AI6" t="n">
-        <v>4242.17</v>
+        <v>8499.33</v>
       </c>
       <c r="AJ6" t="n">
-        <v>4362.09</v>
+        <v>8739.17</v>
       </c>
       <c r="AK6" t="n">
-        <v>4497</v>
+        <v>8994</v>
       </c>
     </row>
     <row r="7">
@@ -1685,112 +1844,112 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="C7" t="n">
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="D7" t="n">
-        <v>662.5</v>
+        <v>1325</v>
       </c>
       <c r="E7" t="n">
-        <v>862.5</v>
+        <v>1725</v>
       </c>
       <c r="F7" t="n">
-        <v>1062.5</v>
+        <v>2125</v>
       </c>
       <c r="G7" t="n">
-        <v>1275</v>
+        <v>2550</v>
       </c>
       <c r="H7" t="n">
-        <v>1475</v>
+        <v>2950</v>
       </c>
       <c r="I7" t="n">
-        <v>1687.5</v>
+        <v>3375</v>
       </c>
       <c r="J7" t="n">
-        <v>1887.5</v>
+        <v>3775</v>
       </c>
       <c r="K7" t="n">
-        <v>2087.5</v>
+        <v>4175</v>
       </c>
       <c r="L7" t="n">
-        <v>2300</v>
+        <v>4600</v>
       </c>
       <c r="M7" t="n">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="N7" t="n">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="O7" t="n">
-        <v>2725</v>
+        <v>6375</v>
       </c>
       <c r="P7" t="n">
-        <v>2950</v>
+        <v>7725</v>
       </c>
       <c r="Q7" t="n">
-        <v>3187.5</v>
+        <v>9100</v>
       </c>
       <c r="R7" t="n">
-        <v>3412.5</v>
+        <v>10450</v>
       </c>
       <c r="S7" t="n">
-        <v>3637.5</v>
+        <v>11825</v>
       </c>
       <c r="T7" t="n">
-        <v>3862.5</v>
+        <v>13175</v>
       </c>
       <c r="U7" t="n">
-        <v>4087.5</v>
+        <v>14550</v>
       </c>
       <c r="V7" t="n">
-        <v>4312.5</v>
+        <v>15900</v>
       </c>
       <c r="W7" t="n">
-        <v>4550</v>
+        <v>17275</v>
       </c>
       <c r="X7" t="n">
-        <v>4775</v>
+        <v>18625</v>
       </c>
       <c r="Y7" t="n">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="Z7" t="n">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="AA7" t="n">
-        <v>5450</v>
+        <v>22725</v>
       </c>
       <c r="AB7" t="n">
-        <v>5912.5</v>
+        <v>25450</v>
       </c>
       <c r="AC7" t="n">
-        <v>6362.5</v>
+        <v>28175</v>
       </c>
       <c r="AD7" t="n">
-        <v>6812.5</v>
+        <v>30900</v>
       </c>
       <c r="AE7" t="n">
-        <v>7275</v>
+        <v>33625</v>
       </c>
       <c r="AF7" t="n">
-        <v>7725</v>
+        <v>36375</v>
       </c>
       <c r="AG7" t="n">
-        <v>8187.5</v>
+        <v>39100</v>
       </c>
       <c r="AH7" t="n">
-        <v>8637.5</v>
+        <v>41825</v>
       </c>
       <c r="AI7" t="n">
-        <v>9087.5</v>
+        <v>44550</v>
       </c>
       <c r="AJ7" t="n">
-        <v>9550</v>
+        <v>47275</v>
       </c>
       <c r="AK7" t="n">
-        <v>10000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="8">
@@ -1800,112 +1959,112 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>399.9</v>
+        <v>649.9</v>
       </c>
       <c r="C8" t="n">
-        <v>719.8200000000001</v>
+        <v>1169.82</v>
       </c>
       <c r="D8" t="n">
-        <v>1052.24</v>
+        <v>1729.73</v>
       </c>
       <c r="E8" t="n">
-        <v>1372.16</v>
+        <v>2249.65</v>
       </c>
       <c r="F8" t="n">
-        <v>1707.07</v>
+        <v>2769.57</v>
       </c>
       <c r="G8" t="n">
-        <v>2039.49</v>
+        <v>3314.49</v>
       </c>
       <c r="H8" t="n">
-        <v>2359.41</v>
+        <v>3849.4</v>
       </c>
       <c r="I8" t="n">
-        <v>2706.82</v>
+        <v>4394.32</v>
       </c>
       <c r="J8" t="n">
-        <v>3026.74</v>
+        <v>4914.24</v>
       </c>
       <c r="K8" t="n">
-        <v>3346.66</v>
+        <v>5449.15</v>
       </c>
       <c r="L8" t="n">
-        <v>3679.08</v>
+        <v>5994.07</v>
       </c>
       <c r="M8" t="n">
-        <v>4013.99</v>
+        <v>6513.99</v>
       </c>
       <c r="N8" t="n">
-        <v>4133.91</v>
+        <v>7458.36</v>
       </c>
       <c r="O8" t="n">
-        <v>4478.83</v>
+        <v>9028.23</v>
       </c>
       <c r="P8" t="n">
-        <v>4838.74</v>
+        <v>10558.11</v>
       </c>
       <c r="Q8" t="n">
-        <v>5196.16</v>
+        <v>12112.99</v>
       </c>
       <c r="R8" t="n">
-        <v>5541.08</v>
+        <v>13657.86</v>
       </c>
       <c r="S8" t="n">
-        <v>5886</v>
+        <v>15212.74</v>
       </c>
       <c r="T8" t="n">
-        <v>6245.91</v>
+        <v>16757.61</v>
       </c>
       <c r="U8" t="n">
-        <v>6590.83</v>
+        <v>18312.49</v>
       </c>
       <c r="V8" t="n">
-        <v>6935.75</v>
+        <v>19857.36</v>
       </c>
       <c r="W8" t="n">
-        <v>7308.16</v>
+        <v>21412.24</v>
       </c>
       <c r="X8" t="n">
-        <v>7653.08</v>
+        <v>22942.12</v>
       </c>
       <c r="Y8" t="n">
-        <v>7998</v>
+        <v>24511.99</v>
       </c>
       <c r="Z8" t="n">
-        <v>8117.92</v>
+        <v>26265.82</v>
       </c>
       <c r="AA8" t="n">
-        <v>8702.83</v>
+        <v>29230.66</v>
       </c>
       <c r="AB8" t="n">
-        <v>9285.25</v>
+        <v>32210.49</v>
       </c>
       <c r="AC8" t="n">
-        <v>9855.17</v>
+        <v>35175.33</v>
       </c>
       <c r="AD8" t="n">
-        <v>10440.08</v>
+        <v>38155.16</v>
       </c>
       <c r="AE8" t="n">
-        <v>11022.5</v>
+        <v>41134.99</v>
       </c>
       <c r="AF8" t="n">
-        <v>11592.42</v>
+        <v>44124.83</v>
       </c>
       <c r="AG8" t="n">
-        <v>12174.84</v>
+        <v>47104.66</v>
       </c>
       <c r="AH8" t="n">
-        <v>12759.75</v>
+        <v>50069.5</v>
       </c>
       <c r="AI8" t="n">
-        <v>13329.67</v>
+        <v>53049.33</v>
       </c>
       <c r="AJ8" t="n">
-        <v>13912.09</v>
+        <v>56014.17</v>
       </c>
       <c r="AK8" t="n">
-        <v>14497</v>
+        <v>58994</v>
       </c>
     </row>
     <row r="9">
@@ -2490,112 +2649,112 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-5433.43</v>
+        <v>-5666.75</v>
       </c>
       <c r="C14" t="n">
-        <v>-5113.51</v>
+        <v>-5146.83</v>
       </c>
       <c r="D14" t="n">
-        <v>-4781.09</v>
+        <v>-4586.92</v>
       </c>
       <c r="E14" t="n">
-        <v>-4461.17</v>
+        <v>-4067</v>
       </c>
       <c r="F14" t="n">
-        <v>-4126.26</v>
+        <v>-3547.08</v>
       </c>
       <c r="G14" t="n">
-        <v>-3793.84</v>
+        <v>-3002.16</v>
       </c>
       <c r="H14" t="n">
-        <v>-3473.92</v>
+        <v>-2467.25</v>
       </c>
       <c r="I14" t="n">
-        <v>-3126.51</v>
+        <v>-1922.33</v>
       </c>
       <c r="J14" t="n">
-        <v>-2806.59</v>
+        <v>-1402.41</v>
       </c>
       <c r="K14" t="n">
-        <v>-2486.67</v>
+        <v>-867.5</v>
       </c>
       <c r="L14" t="n">
-        <v>-2154.25</v>
+        <v>-322.58</v>
       </c>
       <c r="M14" t="n">
-        <v>-1819.34</v>
+        <v>197.34</v>
       </c>
       <c r="N14" t="n">
-        <v>-4699.42</v>
+        <v>-1858.29</v>
       </c>
       <c r="O14" t="n">
-        <v>-4354.5</v>
+        <v>-288.42</v>
       </c>
       <c r="P14" t="n">
-        <v>-3994.59</v>
+        <v>1241.46</v>
       </c>
       <c r="Q14" t="n">
-        <v>-3637.17</v>
+        <v>2796.34</v>
       </c>
       <c r="R14" t="n">
-        <v>-3292.25</v>
+        <v>4341.21</v>
       </c>
       <c r="S14" t="n">
-        <v>-2947.33</v>
+        <v>5896.09</v>
       </c>
       <c r="T14" t="n">
-        <v>-2587.42</v>
+        <v>7440.96</v>
       </c>
       <c r="U14" t="n">
-        <v>-2242.5</v>
+        <v>8995.84</v>
       </c>
       <c r="V14" t="n">
-        <v>-1897.58</v>
+        <v>10540.71</v>
       </c>
       <c r="W14" t="n">
-        <v>-1525.17</v>
+        <v>12095.59</v>
       </c>
       <c r="X14" t="n">
-        <v>-1180.25</v>
+        <v>13625.47</v>
       </c>
       <c r="Y14" t="n">
-        <v>-835.33</v>
+        <v>15195.34</v>
       </c>
       <c r="Z14" t="n">
-        <v>-715.41</v>
+        <v>16949.17</v>
       </c>
       <c r="AA14" t="n">
-        <v>-130.5</v>
+        <v>19914.01</v>
       </c>
       <c r="AB14" t="n">
-        <v>451.92</v>
+        <v>22893.84</v>
       </c>
       <c r="AC14" t="n">
-        <v>1021.84</v>
+        <v>25858.68</v>
       </c>
       <c r="AD14" t="n">
-        <v>1606.75</v>
+        <v>28838.51</v>
       </c>
       <c r="AE14" t="n">
-        <v>2189.17</v>
+        <v>31818.34</v>
       </c>
       <c r="AF14" t="n">
-        <v>2759.09</v>
+        <v>34808.18</v>
       </c>
       <c r="AG14" t="n">
-        <v>3341.51</v>
+        <v>37788.01</v>
       </c>
       <c r="AH14" t="n">
-        <v>3926.42</v>
+        <v>40752.85</v>
       </c>
       <c r="AI14" t="n">
-        <v>4496.34</v>
+        <v>43732.68</v>
       </c>
       <c r="AJ14" t="n">
-        <v>5078.76</v>
+        <v>46697.52</v>
       </c>
       <c r="AK14" t="n">
-        <v>5663.67</v>
+        <v>49677.35</v>
       </c>
     </row>
     <row r="15">
@@ -2605,112 +2764,342 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>104566.57</v>
+        <v>44333.25</v>
       </c>
       <c r="C15" t="n">
-        <v>99453.05</v>
+        <v>39186.41</v>
       </c>
       <c r="D15" t="n">
-        <v>94671.96000000001</v>
+        <v>34599.49</v>
       </c>
       <c r="E15" t="n">
-        <v>90210.78999999999</v>
+        <v>30532.49</v>
       </c>
       <c r="F15" t="n">
-        <v>86084.52</v>
+        <v>26985.4</v>
       </c>
       <c r="G15" t="n">
-        <v>82290.67999999999</v>
+        <v>23983.24</v>
       </c>
       <c r="H15" t="n">
-        <v>78816.75999999999</v>
+        <v>21515.99</v>
       </c>
       <c r="I15" t="n">
-        <v>75690.24000000001</v>
+        <v>19593.65</v>
       </c>
       <c r="J15" t="n">
-        <v>72883.64999999999</v>
+        <v>18191.24</v>
       </c>
       <c r="K15" t="n">
-        <v>70396.98</v>
+        <v>17323.74</v>
       </c>
       <c r="L15" t="n">
-        <v>68242.72</v>
+        <v>17001.15</v>
       </c>
       <c r="M15" t="n">
-        <v>66423.38</v>
+        <v>17198.49</v>
       </c>
       <c r="N15" t="n">
-        <v>61723.96</v>
+        <v>15340.2</v>
       </c>
       <c r="O15" t="n">
-        <v>57369.45</v>
+        <v>15051.77</v>
       </c>
       <c r="P15" t="n">
-        <v>53374.86</v>
+        <v>16293.23</v>
       </c>
       <c r="Q15" t="n">
-        <v>49737.69</v>
+        <v>19089.57</v>
       </c>
       <c r="R15" t="n">
-        <v>46445.43</v>
+        <v>23430.77</v>
       </c>
       <c r="S15" t="n">
-        <v>43498.1</v>
+        <v>29326.86</v>
       </c>
       <c r="T15" t="n">
-        <v>40910.68</v>
+        <v>36767.82</v>
       </c>
       <c r="U15" t="n">
-        <v>38668.17</v>
+        <v>45763.65</v>
       </c>
       <c r="V15" t="n">
-        <v>36770.59</v>
+        <v>56304.36</v>
       </c>
       <c r="W15" t="n">
-        <v>35245.42</v>
+        <v>68399.95</v>
       </c>
       <c r="X15" t="n">
-        <v>34065.16</v>
+        <v>82025.41</v>
       </c>
       <c r="Y15" t="n">
-        <v>33229.83</v>
+        <v>97220.75</v>
       </c>
       <c r="Z15" t="n">
-        <v>32514.42</v>
+        <v>114169.92</v>
       </c>
       <c r="AA15" t="n">
-        <v>32383.91</v>
+        <v>134083.92</v>
       </c>
       <c r="AB15" t="n">
-        <v>32835.83</v>
+        <v>156977.76</v>
       </c>
       <c r="AC15" t="n">
-        <v>33857.67</v>
+        <v>182836.44</v>
       </c>
       <c r="AD15" t="n">
-        <v>35464.41</v>
+        <v>211674.94</v>
       </c>
       <c r="AE15" t="n">
-        <v>37653.58</v>
+        <v>243493.28</v>
       </c>
       <c r="AF15" t="n">
-        <v>40412.67</v>
+        <v>278301.46</v>
       </c>
       <c r="AG15" t="n">
-        <v>43754.17</v>
+        <v>316089.46</v>
       </c>
       <c r="AH15" t="n">
-        <v>47680.59</v>
+        <v>356842.31</v>
       </c>
       <c r="AI15" t="n">
-        <v>52176.93</v>
+        <v>400574.99</v>
       </c>
       <c r="AJ15" t="n">
-        <v>57255.68</v>
+        <v>447272.5</v>
       </c>
       <c r="AK15" t="n">
-        <v>62919.35</v>
+        <v>496949.85</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Loan Repayment €</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="C16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="D16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="E16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="F16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="G16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="H16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="I16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="J16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="K16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="L16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="M16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="N16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="O16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="P16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="R16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="S16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="T16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="U16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="V16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="W16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="X16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>483.32</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>483.32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Reserves €</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>25000</v>
+      </c>
+      <c r="C17" t="n">
+        <v/>
+      </c>
+      <c r="D17" t="n">
+        <v/>
+      </c>
+      <c r="E17" t="n">
+        <v/>
+      </c>
+      <c r="F17" t="n">
+        <v/>
+      </c>
+      <c r="G17" t="n">
+        <v/>
+      </c>
+      <c r="H17" t="n">
+        <v/>
+      </c>
+      <c r="I17" t="n">
+        <v/>
+      </c>
+      <c r="J17" t="n">
+        <v/>
+      </c>
+      <c r="K17" t="n">
+        <v/>
+      </c>
+      <c r="L17" t="n">
+        <v/>
+      </c>
+      <c r="M17" t="n">
+        <v/>
+      </c>
+      <c r="N17" t="n">
+        <v/>
+      </c>
+      <c r="O17" t="n">
+        <v/>
+      </c>
+      <c r="P17" t="n">
+        <v/>
+      </c>
+      <c r="Q17" t="n">
+        <v/>
+      </c>
+      <c r="R17" t="n">
+        <v/>
+      </c>
+      <c r="S17" t="n">
+        <v/>
+      </c>
+      <c r="T17" t="n">
+        <v/>
+      </c>
+      <c r="U17" t="n">
+        <v/>
+      </c>
+      <c r="V17" t="n">
+        <v/>
+      </c>
+      <c r="W17" t="n">
+        <v/>
+      </c>
+      <c r="X17" t="n">
+        <v/>
+      </c>
+      <c r="Y17" t="n">
+        <v/>
+      </c>
+      <c r="Z17" t="n">
+        <v/>
+      </c>
+      <c r="AA17" t="n">
+        <v/>
+      </c>
+      <c r="AB17" t="n">
+        <v/>
+      </c>
+      <c r="AC17" t="n">
+        <v/>
+      </c>
+      <c r="AD17" t="n">
+        <v/>
+      </c>
+      <c r="AE17" t="n">
+        <v/>
+      </c>
+      <c r="AF17" t="n">
+        <v/>
+      </c>
+      <c r="AG17" t="n">
+        <v/>
+      </c>
+      <c r="AH17" t="n">
+        <v/>
+      </c>
+      <c r="AI17" t="n">
+        <v/>
+      </c>
+      <c r="AJ17" t="n">
+        <v/>
+      </c>
+      <c r="AK17" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2725,7 +3114,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2736,136 +3125,75 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>Metric</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Total Revenue €</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Total Expenses €</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Net Cash Flow €</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Ending Cash €</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026</t>
+          <t>Monthly Loan Repayment €</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>26423.38</v>
-      </c>
-      <c r="C2" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-43576.62</v>
-      </c>
-      <c r="E2" t="n">
-        <v>66423.38</v>
+        <v>483.32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2027</t>
+          <t>Total Loan Paid in 36m €</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72806.45</v>
-      </c>
-      <c r="C3" t="n">
-        <v>106000</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-33193.55</v>
-      </c>
-      <c r="E3" t="n">
-        <v>33229.83</v>
+        <v>17399.52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2028</t>
+          <t>Ending Cash Dec-28 €</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>135689.52</v>
-      </c>
-      <c r="C4" t="n">
-        <v>106000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>29689.52</v>
-      </c>
-      <c r="E4" t="n">
-        <v>62919.35</v>
+        <v>496949.85</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Lowest Cash Month</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Feb-27</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Key Highlights</t>
-        </is>
+          <t>Lowest Cash Balance €</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>15051.77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Breakeven Month</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Mar-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Lowest Cash Month</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Feb-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Lowest Cash Balance €</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>32383.91</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Ending Cash Dec-28 €</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>62919.35</v>
+          <t>Reserves Allocated €</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>25000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update financial plan for 6% amortizing loan
</commit_message>
<xml_diff>
--- a/public/data/consultantcloud_36m_financial_plan.xlsx
+++ b/public/data/consultantcloud_36m_financial_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Financial Plan" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Financial Plan" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -126,13 +126,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -150,14 +150,14 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -177,14 +177,14 @@
           <idx val="1"/>
           <order val="1"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -204,14 +204,14 @@
           <idx val="2"/>
           <order val="2"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -239,8 +239,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -266,8 +266,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -293,13 +293,13 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -317,14 +317,14 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -344,14 +344,14 @@
           <idx val="1"/>
           <order val="1"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -371,14 +371,14 @@
           <idx val="2"/>
           <order val="2"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -398,14 +398,14 @@
           <idx val="3"/>
           <order val="3"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -425,14 +425,14 @@
           <idx val="4"/>
           <order val="4"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -452,14 +452,14 @@
           <idx val="5"/>
           <order val="5"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -479,14 +479,14 @@
           <idx val="6"/>
           <order val="6"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -506,14 +506,14 @@
           <idx val="7"/>
           <order val="7"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -541,8 +541,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -568,8 +568,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -595,13 +595,13 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -619,14 +619,14 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -654,8 +654,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -681,8 +681,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -708,7 +708,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>1</col>
@@ -723,9 +723,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -745,9 +745,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -767,9 +767,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1616,111 +1616,6 @@
       <c r="B5" t="n">
         <v>50000</v>
       </c>
-      <c r="C5" t="n">
-        <v/>
-      </c>
-      <c r="D5" t="n">
-        <v/>
-      </c>
-      <c r="E5" t="n">
-        <v/>
-      </c>
-      <c r="F5" t="n">
-        <v/>
-      </c>
-      <c r="G5" t="n">
-        <v/>
-      </c>
-      <c r="H5" t="n">
-        <v/>
-      </c>
-      <c r="I5" t="n">
-        <v/>
-      </c>
-      <c r="J5" t="n">
-        <v/>
-      </c>
-      <c r="K5" t="n">
-        <v/>
-      </c>
-      <c r="L5" t="n">
-        <v/>
-      </c>
-      <c r="M5" t="n">
-        <v/>
-      </c>
-      <c r="N5" t="n">
-        <v/>
-      </c>
-      <c r="O5" t="n">
-        <v/>
-      </c>
-      <c r="P5" t="n">
-        <v/>
-      </c>
-      <c r="Q5" t="n">
-        <v/>
-      </c>
-      <c r="R5" t="n">
-        <v/>
-      </c>
-      <c r="S5" t="n">
-        <v/>
-      </c>
-      <c r="T5" t="n">
-        <v/>
-      </c>
-      <c r="U5" t="n">
-        <v/>
-      </c>
-      <c r="V5" t="n">
-        <v/>
-      </c>
-      <c r="W5" t="n">
-        <v/>
-      </c>
-      <c r="X5" t="n">
-        <v/>
-      </c>
-      <c r="Y5" t="n">
-        <v/>
-      </c>
-      <c r="Z5" t="n">
-        <v/>
-      </c>
-      <c r="AA5" t="n">
-        <v/>
-      </c>
-      <c r="AB5" t="n">
-        <v/>
-      </c>
-      <c r="AC5" t="n">
-        <v/>
-      </c>
-      <c r="AD5" t="n">
-        <v/>
-      </c>
-      <c r="AE5" t="n">
-        <v/>
-      </c>
-      <c r="AF5" t="n">
-        <v/>
-      </c>
-      <c r="AG5" t="n">
-        <v/>
-      </c>
-      <c r="AH5" t="n">
-        <v/>
-      </c>
-      <c r="AI5" t="n">
-        <v/>
-      </c>
-      <c r="AJ5" t="n">
-        <v/>
-      </c>
-      <c r="AK5" t="n">
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2534,112 +2429,112 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="C13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="D13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="E13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="F13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="G13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="H13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="I13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="J13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="K13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="L13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="M13" t="n">
-        <v>5833.33</v>
+        <v>6799.97</v>
       </c>
       <c r="N13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="O13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="P13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="Q13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="R13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="S13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="T13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="U13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="V13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="W13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="X13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="Y13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="Z13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AA13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AB13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AC13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AD13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AE13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AF13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AG13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AH13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AI13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AJ13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
       <c r="AK13" t="n">
-        <v>8833.33</v>
+        <v>9799.969999999999</v>
       </c>
     </row>
     <row r="14">
@@ -2649,112 +2544,112 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-5666.75</v>
+        <v>-6150.07</v>
       </c>
       <c r="C14" t="n">
-        <v>-5146.83</v>
+        <v>-5630.15</v>
       </c>
       <c r="D14" t="n">
-        <v>-4586.92</v>
+        <v>-5070.24</v>
       </c>
       <c r="E14" t="n">
-        <v>-4067</v>
+        <v>-4550.32</v>
       </c>
       <c r="F14" t="n">
-        <v>-3547.08</v>
+        <v>-4030.4</v>
       </c>
       <c r="G14" t="n">
-        <v>-3002.16</v>
+        <v>-3485.48</v>
       </c>
       <c r="H14" t="n">
-        <v>-2467.25</v>
+        <v>-2950.57</v>
       </c>
       <c r="I14" t="n">
-        <v>-1922.33</v>
+        <v>-2405.65</v>
       </c>
       <c r="J14" t="n">
-        <v>-1402.41</v>
+        <v>-1885.73</v>
       </c>
       <c r="K14" t="n">
-        <v>-867.5</v>
+        <v>-1350.82</v>
       </c>
       <c r="L14" t="n">
-        <v>-322.58</v>
+        <v>-805.9</v>
       </c>
       <c r="M14" t="n">
-        <v>197.34</v>
+        <v>-285.98</v>
       </c>
       <c r="N14" t="n">
-        <v>-1858.29</v>
+        <v>-2341.61</v>
       </c>
       <c r="O14" t="n">
-        <v>-288.42</v>
+        <v>-771.74</v>
       </c>
       <c r="P14" t="n">
-        <v>1241.46</v>
+        <v>758.14</v>
       </c>
       <c r="Q14" t="n">
-        <v>2796.34</v>
+        <v>2313.02</v>
       </c>
       <c r="R14" t="n">
-        <v>4341.21</v>
+        <v>3857.89</v>
       </c>
       <c r="S14" t="n">
-        <v>5896.09</v>
+        <v>5412.77</v>
       </c>
       <c r="T14" t="n">
-        <v>7440.96</v>
+        <v>6957.64</v>
       </c>
       <c r="U14" t="n">
-        <v>8995.84</v>
+        <v>8512.52</v>
       </c>
       <c r="V14" t="n">
-        <v>10540.71</v>
+        <v>10057.39</v>
       </c>
       <c r="W14" t="n">
-        <v>12095.59</v>
+        <v>11612.27</v>
       </c>
       <c r="X14" t="n">
-        <v>13625.47</v>
+        <v>13142.15</v>
       </c>
       <c r="Y14" t="n">
-        <v>15195.34</v>
+        <v>14712.02</v>
       </c>
       <c r="Z14" t="n">
-        <v>16949.17</v>
+        <v>16465.85</v>
       </c>
       <c r="AA14" t="n">
-        <v>19914.01</v>
+        <v>19430.69</v>
       </c>
       <c r="AB14" t="n">
-        <v>22893.84</v>
+        <v>22410.52</v>
       </c>
       <c r="AC14" t="n">
-        <v>25858.68</v>
+        <v>25375.36</v>
       </c>
       <c r="AD14" t="n">
-        <v>28838.51</v>
+        <v>28355.19</v>
       </c>
       <c r="AE14" t="n">
-        <v>31818.34</v>
+        <v>31335.02</v>
       </c>
       <c r="AF14" t="n">
-        <v>34808.18</v>
+        <v>34324.86</v>
       </c>
       <c r="AG14" t="n">
-        <v>37788.01</v>
+        <v>37304.69</v>
       </c>
       <c r="AH14" t="n">
-        <v>40752.85</v>
+        <v>40269.53</v>
       </c>
       <c r="AI14" t="n">
-        <v>43732.68</v>
+        <v>43249.36</v>
       </c>
       <c r="AJ14" t="n">
-        <v>46697.52</v>
+        <v>46214.2</v>
       </c>
       <c r="AK14" t="n">
-        <v>49677.35</v>
+        <v>49194.03</v>
       </c>
     </row>
     <row r="15">
@@ -2764,112 +2659,112 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>44333.25</v>
+        <v>43849.93</v>
       </c>
       <c r="C15" t="n">
-        <v>39186.41</v>
+        <v>38219.78</v>
       </c>
       <c r="D15" t="n">
-        <v>34599.49</v>
+        <v>33149.54</v>
       </c>
       <c r="E15" t="n">
-        <v>30532.49</v>
+        <v>28599.22</v>
       </c>
       <c r="F15" t="n">
-        <v>26985.4</v>
+        <v>24568.82</v>
       </c>
       <c r="G15" t="n">
-        <v>23983.24</v>
+        <v>21083.34</v>
       </c>
       <c r="H15" t="n">
-        <v>21515.99</v>
+        <v>18132.77</v>
       </c>
       <c r="I15" t="n">
-        <v>19593.65</v>
+        <v>15727.12</v>
       </c>
       <c r="J15" t="n">
-        <v>18191.24</v>
+        <v>13841.39</v>
       </c>
       <c r="K15" t="n">
-        <v>17323.74</v>
+        <v>12490.57</v>
       </c>
       <c r="L15" t="n">
-        <v>17001.15</v>
+        <v>11684.67</v>
       </c>
       <c r="M15" t="n">
-        <v>17198.49</v>
+        <v>11398.69</v>
       </c>
       <c r="N15" t="n">
-        <v>15340.2</v>
+        <v>9057.08</v>
       </c>
       <c r="O15" t="n">
-        <v>15051.77</v>
+        <v>8285.34</v>
       </c>
       <c r="P15" t="n">
-        <v>16293.23</v>
+        <v>9043.48</v>
       </c>
       <c r="Q15" t="n">
-        <v>19089.57</v>
+        <v>11356.5</v>
       </c>
       <c r="R15" t="n">
-        <v>23430.77</v>
+        <v>15214.39</v>
       </c>
       <c r="S15" t="n">
-        <v>29326.86</v>
+        <v>20627.16</v>
       </c>
       <c r="T15" t="n">
-        <v>36767.82</v>
+        <v>27584.8</v>
       </c>
       <c r="U15" t="n">
-        <v>45763.65</v>
+        <v>36097.32</v>
       </c>
       <c r="V15" t="n">
-        <v>56304.36</v>
+        <v>46154.71</v>
       </c>
       <c r="W15" t="n">
-        <v>68399.95</v>
+        <v>57766.98</v>
       </c>
       <c r="X15" t="n">
-        <v>82025.41</v>
+        <v>70909.13</v>
       </c>
       <c r="Y15" t="n">
-        <v>97220.75</v>
+        <v>85621.14999999999</v>
       </c>
       <c r="Z15" t="n">
-        <v>114169.92</v>
+        <v>102087</v>
       </c>
       <c r="AA15" t="n">
-        <v>134083.92</v>
+        <v>121517.69</v>
       </c>
       <c r="AB15" t="n">
-        <v>156977.76</v>
+        <v>143928.21</v>
       </c>
       <c r="AC15" t="n">
-        <v>182836.44</v>
+        <v>169303.57</v>
       </c>
       <c r="AD15" t="n">
-        <v>211674.94</v>
+        <v>197658.76</v>
       </c>
       <c r="AE15" t="n">
-        <v>243493.28</v>
+        <v>228993.78</v>
       </c>
       <c r="AF15" t="n">
-        <v>278301.46</v>
+        <v>263318.64</v>
       </c>
       <c r="AG15" t="n">
-        <v>316089.46</v>
+        <v>300623.33</v>
       </c>
       <c r="AH15" t="n">
-        <v>356842.31</v>
+        <v>340892.86</v>
       </c>
       <c r="AI15" t="n">
-        <v>400574.99</v>
+        <v>384142.22</v>
       </c>
       <c r="AJ15" t="n">
-        <v>447272.5</v>
+        <v>430356.42</v>
       </c>
       <c r="AK15" t="n">
-        <v>496949.85</v>
+        <v>479550.45</v>
       </c>
     </row>
     <row r="16">
@@ -2879,112 +2774,112 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="C16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="D16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="E16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="F16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="G16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="H16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="I16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="J16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="K16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="L16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="M16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="N16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="O16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="P16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="Q16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="R16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="S16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="T16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="U16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="V16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="W16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="X16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="Y16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="Z16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AA16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AB16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AC16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AD16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AE16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AF16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AG16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AH16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AI16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AJ16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
       <c r="AK16" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
     </row>
     <row r="17">
@@ -2995,111 +2890,6 @@
       </c>
       <c r="B17" t="n">
         <v>25000</v>
-      </c>
-      <c r="C17" t="n">
-        <v/>
-      </c>
-      <c r="D17" t="n">
-        <v/>
-      </c>
-      <c r="E17" t="n">
-        <v/>
-      </c>
-      <c r="F17" t="n">
-        <v/>
-      </c>
-      <c r="G17" t="n">
-        <v/>
-      </c>
-      <c r="H17" t="n">
-        <v/>
-      </c>
-      <c r="I17" t="n">
-        <v/>
-      </c>
-      <c r="J17" t="n">
-        <v/>
-      </c>
-      <c r="K17" t="n">
-        <v/>
-      </c>
-      <c r="L17" t="n">
-        <v/>
-      </c>
-      <c r="M17" t="n">
-        <v/>
-      </c>
-      <c r="N17" t="n">
-        <v/>
-      </c>
-      <c r="O17" t="n">
-        <v/>
-      </c>
-      <c r="P17" t="n">
-        <v/>
-      </c>
-      <c r="Q17" t="n">
-        <v/>
-      </c>
-      <c r="R17" t="n">
-        <v/>
-      </c>
-      <c r="S17" t="n">
-        <v/>
-      </c>
-      <c r="T17" t="n">
-        <v/>
-      </c>
-      <c r="U17" t="n">
-        <v/>
-      </c>
-      <c r="V17" t="n">
-        <v/>
-      </c>
-      <c r="W17" t="n">
-        <v/>
-      </c>
-      <c r="X17" t="n">
-        <v/>
-      </c>
-      <c r="Y17" t="n">
-        <v/>
-      </c>
-      <c r="Z17" t="n">
-        <v/>
-      </c>
-      <c r="AA17" t="n">
-        <v/>
-      </c>
-      <c r="AB17" t="n">
-        <v/>
-      </c>
-      <c r="AC17" t="n">
-        <v/>
-      </c>
-      <c r="AD17" t="n">
-        <v/>
-      </c>
-      <c r="AE17" t="n">
-        <v/>
-      </c>
-      <c r="AF17" t="n">
-        <v/>
-      </c>
-      <c r="AG17" t="n">
-        <v/>
-      </c>
-      <c r="AH17" t="n">
-        <v/>
-      </c>
-      <c r="AI17" t="n">
-        <v/>
-      </c>
-      <c r="AJ17" t="n">
-        <v/>
-      </c>
-      <c r="AK17" t="n">
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -3141,7 +2931,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>483.32</v>
+        <v>966.64</v>
       </c>
     </row>
     <row r="3">
@@ -3151,7 +2941,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17399.52</v>
+        <v>34799.04</v>
       </c>
     </row>
     <row r="4">
@@ -3161,7 +2951,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>496949.85</v>
+        <v>479550.45</v>
       </c>
     </row>
     <row r="5">
@@ -3183,7 +2973,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>15051.77</v>
+        <v>8285.34</v>
       </c>
     </row>
     <row r="7">

</xml_diff>